<commit_message>
Task 3 Setup, Model Training and Power BI improvements
</commit_message>
<xml_diff>
--- a/RESULTS/LeaderBoard.xlsx
+++ b/RESULTS/LeaderBoard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbowc\Documents\GitHub\EnergyCatapultPresumedOpenDataChallange-\RESULTS\task1Submission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbowc\Documents\GitHub\EnergyCatapultPresumedOpenDataChallange-\RESULTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2DF954-13AF-4D4D-B93B-FDB084483589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1015B34E-9942-42ED-8FEC-02DF6725EAE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3408" yWindow="1404" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="average_scores_task1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="74">
   <si>
     <t>Team Name</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>vega</t>
+  </si>
+  <si>
+    <t>Batteries_Included</t>
+  </si>
+  <si>
+    <t>WattSmoothoperator</t>
   </si>
 </sst>
 </file>
@@ -1138,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:L130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48:L90"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4622,6 +4628,1526 @@
         <v>4.0461639743573787</v>
       </c>
     </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A91" s="12">
+        <v>2</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91">
+        <v>83.953985769261706</v>
+      </c>
+      <c r="E91">
+        <v>104.167420011128</v>
+      </c>
+      <c r="F91">
+        <v>73.700990499707402</v>
+      </c>
+      <c r="G91">
+        <v>90.950629759421403</v>
+      </c>
+      <c r="H91">
+        <v>66.390539751659006</v>
+      </c>
+      <c r="I91">
+        <v>65.005496218687298</v>
+      </c>
+      <c r="J91">
+        <v>76.110335307711097</v>
+      </c>
+      <c r="K91" s="1">
+        <v>80.039913902510847</v>
+      </c>
+      <c r="L91" s="1">
+        <v>80.039913902510847</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A92" s="12">
+        <v>2</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D92">
+        <v>85.743333333333297</v>
+      </c>
+      <c r="E92">
+        <v>108.126315789473</v>
+      </c>
+      <c r="F92">
+        <v>63.803474366116802</v>
+      </c>
+      <c r="G92">
+        <v>95.308641975308603</v>
+      </c>
+      <c r="H92">
+        <v>63.986927083333299</v>
+      </c>
+      <c r="I92">
+        <v>69.883376068375995</v>
+      </c>
+      <c r="J92">
+        <v>69.753275109170204</v>
+      </c>
+      <c r="K92" s="1">
+        <v>79.515049103587316</v>
+      </c>
+      <c r="L92" s="1">
+        <v>79.515049103587316</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A93" s="12">
+        <v>2</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93">
+        <v>82.943128385128503</v>
+      </c>
+      <c r="E93">
+        <v>101.595438852109</v>
+      </c>
+      <c r="F93">
+        <v>74.078186618464599</v>
+      </c>
+      <c r="G93">
+        <v>95.4685258911706</v>
+      </c>
+      <c r="H93">
+        <v>65.937697932616004</v>
+      </c>
+      <c r="I93">
+        <v>66.596706082289501</v>
+      </c>
+      <c r="J93">
+        <v>69.964123270348097</v>
+      </c>
+      <c r="K93" s="1">
+        <v>79.511972433160892</v>
+      </c>
+      <c r="L93" s="1">
+        <v>79.511972433160892</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A94" s="12">
+        <v>2</v>
+      </c>
+      <c r="B94">
+        <v>4</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94">
+        <v>84.1284930792675</v>
+      </c>
+      <c r="E94">
+        <v>99.927817718602</v>
+      </c>
+      <c r="F94">
+        <v>72.793703569017794</v>
+      </c>
+      <c r="G94">
+        <v>98.242227998771099</v>
+      </c>
+      <c r="H94">
+        <v>60.2356496240075</v>
+      </c>
+      <c r="I94">
+        <v>68.844791083870504</v>
+      </c>
+      <c r="J94">
+        <v>71.587787458340998</v>
+      </c>
+      <c r="K94" s="1">
+        <v>79.394352933125347</v>
+      </c>
+      <c r="L94" s="1">
+        <v>79.394352933125347</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A95" s="12">
+        <v>2</v>
+      </c>
+      <c r="B95">
+        <v>5</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D95">
+        <v>85.965354352769495</v>
+      </c>
+      <c r="E95">
+        <v>99.444976242487499</v>
+      </c>
+      <c r="F95">
+        <v>68.327527329884504</v>
+      </c>
+      <c r="G95">
+        <v>93.546576858912303</v>
+      </c>
+      <c r="H95">
+        <v>65.301452065293503</v>
+      </c>
+      <c r="I95">
+        <v>64.428159792816601</v>
+      </c>
+      <c r="J95">
+        <v>71.333599150633901</v>
+      </c>
+      <c r="K95" s="1">
+        <v>78.335377970399691</v>
+      </c>
+      <c r="L95" s="1">
+        <v>78.335377970399691</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A96" s="12">
+        <v>2</v>
+      </c>
+      <c r="B96">
+        <v>6</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D96">
+        <v>85.212102557901503</v>
+      </c>
+      <c r="E96">
+        <v>105.00110254736801</v>
+      </c>
+      <c r="F96">
+        <v>68.864175394238103</v>
+      </c>
+      <c r="G96">
+        <v>92.120201419753002</v>
+      </c>
+      <c r="H96">
+        <v>60.796749213061801</v>
+      </c>
+      <c r="I96">
+        <v>67.222211130377403</v>
+      </c>
+      <c r="J96">
+        <v>68.774270107491105</v>
+      </c>
+      <c r="K96" s="1">
+        <v>78.284401767170138</v>
+      </c>
+      <c r="L96" s="1">
+        <v>78.284401767170138</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A97" s="12">
+        <v>2</v>
+      </c>
+      <c r="B97">
+        <v>7</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D97">
+        <v>88.821294388892497</v>
+      </c>
+      <c r="E97">
+        <v>97.232349473684195</v>
+      </c>
+      <c r="F97">
+        <v>62.706473686288497</v>
+      </c>
+      <c r="G97">
+        <v>93.194740740740698</v>
+      </c>
+      <c r="H97">
+        <v>67.768607892557</v>
+      </c>
+      <c r="I97">
+        <v>66.844981498577496</v>
+      </c>
+      <c r="J97">
+        <v>69.197066591971705</v>
+      </c>
+      <c r="K97" s="1">
+        <v>77.966502038958865</v>
+      </c>
+      <c r="L97" s="1">
+        <v>77.966502038958865</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A98" s="12">
+        <v>2</v>
+      </c>
+      <c r="B98">
+        <v>8</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D98">
+        <v>80.5712747064007</v>
+      </c>
+      <c r="E98">
+        <v>103.78780758181701</v>
+      </c>
+      <c r="F98">
+        <v>63.374245281746802</v>
+      </c>
+      <c r="G98">
+        <v>91.524241575463094</v>
+      </c>
+      <c r="H98">
+        <v>64.410879762743207</v>
+      </c>
+      <c r="I98">
+        <v>66.519522851749102</v>
+      </c>
+      <c r="J98">
+        <v>74.938068215565195</v>
+      </c>
+      <c r="K98" s="1">
+        <v>77.875148567926445</v>
+      </c>
+      <c r="L98" s="1">
+        <v>77.875148567926445</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A99" s="12">
+        <v>2</v>
+      </c>
+      <c r="B99">
+        <v>9</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99">
+        <v>73.3274615727845</v>
+      </c>
+      <c r="E99">
+        <v>99.608460252631602</v>
+      </c>
+      <c r="F99">
+        <v>76.070947885498597</v>
+      </c>
+      <c r="G99">
+        <v>91.427314999999993</v>
+      </c>
+      <c r="H99">
+        <v>62.061523192143497</v>
+      </c>
+      <c r="I99">
+        <v>67.624789852564007</v>
+      </c>
+      <c r="J99">
+        <v>71.584437151576495</v>
+      </c>
+      <c r="K99" s="1">
+        <v>77.386419272456948</v>
+      </c>
+      <c r="L99" s="1">
+        <v>77.386419272456948</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A100" s="12">
+        <v>2</v>
+      </c>
+      <c r="B100">
+        <v>10</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100">
+        <v>87.662008794854202</v>
+      </c>
+      <c r="E100">
+        <v>96.706293903691105</v>
+      </c>
+      <c r="F100">
+        <v>69.569263179693806</v>
+      </c>
+      <c r="G100">
+        <v>84.697530864197503</v>
+      </c>
+      <c r="H100">
+        <v>61.434635416666602</v>
+      </c>
+      <c r="I100">
+        <v>64.489427369159699</v>
+      </c>
+      <c r="J100">
+        <v>72.190203170052797</v>
+      </c>
+      <c r="K100" s="1">
+        <v>76.678480385473677</v>
+      </c>
+      <c r="L100" s="1">
+        <v>76.678480385473677</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A101" s="12">
+        <v>2</v>
+      </c>
+      <c r="B101">
+        <v>11</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D101">
+        <v>85.295616520649105</v>
+      </c>
+      <c r="E101">
+        <v>103.734798351408</v>
+      </c>
+      <c r="F101">
+        <v>64.034148793608793</v>
+      </c>
+      <c r="G101">
+        <v>95.011203721115393</v>
+      </c>
+      <c r="H101">
+        <v>53.441775217137497</v>
+      </c>
+      <c r="I101">
+        <v>66.189250274852</v>
+      </c>
+      <c r="J101">
+        <v>68.806721449196502</v>
+      </c>
+      <c r="K101" s="1">
+        <v>76.64478776113819</v>
+      </c>
+      <c r="L101" s="1">
+        <v>76.64478776113819</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A102" s="12">
+        <v>2</v>
+      </c>
+      <c r="B102">
+        <v>12</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D102">
+        <v>84.8129470986309</v>
+      </c>
+      <c r="E102">
+        <v>95.492842105263193</v>
+      </c>
+      <c r="F102">
+        <v>63.872872420091603</v>
+      </c>
+      <c r="G102">
+        <v>94.450617283950606</v>
+      </c>
+      <c r="H102">
+        <v>62.360067692361099</v>
+      </c>
+      <c r="I102">
+        <v>68.473980182020497</v>
+      </c>
+      <c r="J102">
+        <v>65.377255899563295</v>
+      </c>
+      <c r="K102" s="1">
+        <v>76.405797525983033</v>
+      </c>
+      <c r="L102" s="1">
+        <v>76.405797525983033</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A103" s="12">
+        <v>2</v>
+      </c>
+      <c r="B103">
+        <v>13</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D103">
+        <v>89.418873669214705</v>
+      </c>
+      <c r="E103">
+        <v>103.866028736842</v>
+      </c>
+      <c r="F103">
+        <v>74.960043622719596</v>
+      </c>
+      <c r="G103">
+        <v>93.902803456790096</v>
+      </c>
+      <c r="H103">
+        <v>51.786973124992599</v>
+      </c>
+      <c r="I103">
+        <v>57.213865679154203</v>
+      </c>
+      <c r="J103">
+        <v>61.138819859732301</v>
+      </c>
+      <c r="K103" s="1">
+        <v>76.041058307063636</v>
+      </c>
+      <c r="L103" s="1">
+        <v>76.041058307063636</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A104" s="12">
+        <v>2</v>
+      </c>
+      <c r="B104">
+        <v>14</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104">
+        <v>88.950645564277195</v>
+      </c>
+      <c r="E104">
+        <v>89.291375361716803</v>
+      </c>
+      <c r="F104">
+        <v>57.043796334317101</v>
+      </c>
+      <c r="G104">
+        <v>87.667264821373706</v>
+      </c>
+      <c r="H104">
+        <v>67.157570755005295</v>
+      </c>
+      <c r="I104">
+        <v>69.181797281246105</v>
+      </c>
+      <c r="J104">
+        <v>71.258955800671501</v>
+      </c>
+      <c r="K104" s="1">
+        <v>75.793057988372524</v>
+      </c>
+      <c r="L104" s="1">
+        <v>75.793057988372524</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A105" s="12">
+        <v>2</v>
+      </c>
+      <c r="B105">
+        <v>15</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105">
+        <v>84.395749201565195</v>
+      </c>
+      <c r="E105">
+        <v>96.804654581275599</v>
+      </c>
+      <c r="F105">
+        <v>52.256245292955697</v>
+      </c>
+      <c r="G105">
+        <v>95.449967590383096</v>
+      </c>
+      <c r="H105">
+        <v>62.805725557642198</v>
+      </c>
+      <c r="I105">
+        <v>64.583922521602503</v>
+      </c>
+      <c r="J105">
+        <v>72.942067301922606</v>
+      </c>
+      <c r="K105" s="1">
+        <v>75.605476006763851</v>
+      </c>
+      <c r="L105" s="1">
+        <v>75.605476006763851</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A106" s="12">
+        <v>2</v>
+      </c>
+      <c r="B106">
+        <v>16</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D106">
+        <v>85.561441531353694</v>
+      </c>
+      <c r="E106">
+        <v>101.437473502332</v>
+      </c>
+      <c r="F106">
+        <v>64.327125078855303</v>
+      </c>
+      <c r="G106">
+        <v>95.811642560316102</v>
+      </c>
+      <c r="H106">
+        <v>52.262759212235899</v>
+      </c>
+      <c r="I106">
+        <v>60.048685588947201</v>
+      </c>
+      <c r="J106">
+        <v>67.336723689227895</v>
+      </c>
+      <c r="K106" s="1">
+        <v>75.255121594752595</v>
+      </c>
+      <c r="L106" s="1">
+        <v>75.255121594752595</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A107" s="12">
+        <v>2</v>
+      </c>
+      <c r="B107">
+        <v>17</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107">
+        <v>63.1428375456521</v>
+      </c>
+      <c r="E107">
+        <v>105.347929255322</v>
+      </c>
+      <c r="F107">
+        <v>61.652853184932503</v>
+      </c>
+      <c r="G107">
+        <v>91.949182667347699</v>
+      </c>
+      <c r="H107">
+        <v>63.9092533438888</v>
+      </c>
+      <c r="I107">
+        <v>63.616790559751003</v>
+      </c>
+      <c r="J107">
+        <v>71.052569010468005</v>
+      </c>
+      <c r="K107" s="1">
+        <v>74.381630795337443</v>
+      </c>
+      <c r="L107" s="1">
+        <v>74.381630795337443</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A108" s="12">
+        <v>2</v>
+      </c>
+      <c r="B108">
+        <v>18</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108">
+        <v>79.497566205533502</v>
+      </c>
+      <c r="E108">
+        <v>96.357695196172301</v>
+      </c>
+      <c r="F108">
+        <v>59.046863954487002</v>
+      </c>
+      <c r="G108">
+        <v>89.812463524130195</v>
+      </c>
+      <c r="H108">
+        <v>55.641485771780303</v>
+      </c>
+      <c r="I108">
+        <v>63.568520874773299</v>
+      </c>
+      <c r="J108">
+        <v>69.392805049019799</v>
+      </c>
+      <c r="K108" s="1">
+        <v>73.331057225128049</v>
+      </c>
+      <c r="L108" s="1">
+        <v>73.331057225128049</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A109" s="12">
+        <v>2</v>
+      </c>
+      <c r="B109">
+        <v>19</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D109">
+        <v>88.089434467162306</v>
+      </c>
+      <c r="E109">
+        <v>86.819643443702404</v>
+      </c>
+      <c r="F109">
+        <v>69.393047323701694</v>
+      </c>
+      <c r="G109">
+        <v>75.501693398341899</v>
+      </c>
+      <c r="H109">
+        <v>56.987989264666297</v>
+      </c>
+      <c r="I109">
+        <v>64.747064449101103</v>
+      </c>
+      <c r="J109">
+        <v>67.749029038021902</v>
+      </c>
+      <c r="K109" s="1">
+        <v>72.755414483528227</v>
+      </c>
+      <c r="L109" s="1">
+        <v>72.755414483528227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A110" s="12">
+        <v>2</v>
+      </c>
+      <c r="B110">
+        <v>20</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D110">
+        <v>85.346775824258401</v>
+      </c>
+      <c r="E110">
+        <v>95.224919178947303</v>
+      </c>
+      <c r="F110">
+        <v>48.113460932042699</v>
+      </c>
+      <c r="G110">
+        <v>95.021922592592503</v>
+      </c>
+      <c r="H110">
+        <v>56.12723940115</v>
+      </c>
+      <c r="I110">
+        <v>61.595340552467199</v>
+      </c>
+      <c r="J110">
+        <v>67.168506755282905</v>
+      </c>
+      <c r="K110" s="1">
+        <v>72.656880748105863</v>
+      </c>
+      <c r="L110" s="1">
+        <v>72.656880748105863</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A111" s="12">
+        <v>2</v>
+      </c>
+      <c r="B111">
+        <v>21</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D111">
+        <v>72.857952898550593</v>
+      </c>
+      <c r="E111">
+        <v>102.31578947368401</v>
+      </c>
+      <c r="F111">
+        <v>57.790767990324497</v>
+      </c>
+      <c r="G111">
+        <v>85.864197530864203</v>
+      </c>
+      <c r="H111">
+        <v>60.7753263888888</v>
+      </c>
+      <c r="I111">
+        <v>58.814281502182403</v>
+      </c>
+      <c r="J111">
+        <v>69.610218071347006</v>
+      </c>
+      <c r="K111" s="1">
+        <v>72.575504836548774</v>
+      </c>
+      <c r="L111" s="1">
+        <v>72.575504836548774</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A112" s="12">
+        <v>2</v>
+      </c>
+      <c r="B112">
+        <v>22</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112">
+        <v>85.363206103251997</v>
+      </c>
+      <c r="E112">
+        <v>98.844155747368404</v>
+      </c>
+      <c r="F112">
+        <v>46.018748529899597</v>
+      </c>
+      <c r="G112">
+        <v>91.105537283950596</v>
+      </c>
+      <c r="H112">
+        <v>58.823069307210098</v>
+      </c>
+      <c r="I112">
+        <v>40.5043899106862</v>
+      </c>
+      <c r="J112">
+        <v>75.2576350088071</v>
+      </c>
+      <c r="K112" s="1">
+        <v>70.845248841596288</v>
+      </c>
+      <c r="L112" s="1">
+        <v>70.845248841596288</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A113" s="12">
+        <v>2</v>
+      </c>
+      <c r="B113">
+        <v>23</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D113">
+        <v>80.209975951385204</v>
+      </c>
+      <c r="E113">
+        <v>89.400751124616406</v>
+      </c>
+      <c r="F113">
+        <v>57.099364316405001</v>
+      </c>
+      <c r="G113">
+        <v>69.554226133513893</v>
+      </c>
+      <c r="H113">
+        <v>61.904309537890001</v>
+      </c>
+      <c r="I113">
+        <v>65.307790476166304</v>
+      </c>
+      <c r="J113">
+        <v>70.983553055091505</v>
+      </c>
+      <c r="K113" s="1">
+        <v>70.637138656438324</v>
+      </c>
+      <c r="L113" s="1">
+        <v>70.637138656438324</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A114" s="12">
+        <v>2</v>
+      </c>
+      <c r="B114">
+        <v>24</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D114">
+        <v>89.652259976196007</v>
+      </c>
+      <c r="E114">
+        <v>81.243995133655204</v>
+      </c>
+      <c r="F114">
+        <v>57.1517032500822</v>
+      </c>
+      <c r="G114">
+        <v>73.849604826611099</v>
+      </c>
+      <c r="H114">
+        <v>57.526560805828701</v>
+      </c>
+      <c r="I114">
+        <v>61.0151593360942</v>
+      </c>
+      <c r="J114">
+        <v>72.808781145360101</v>
+      </c>
+      <c r="K114" s="1">
+        <v>70.464009210546791</v>
+      </c>
+      <c r="L114" s="1">
+        <v>70.464009210546791</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A115" s="12">
+        <v>2</v>
+      </c>
+      <c r="B115">
+        <v>25</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D115" s="2">
+        <v>79.110968376293201</v>
+      </c>
+      <c r="E115" s="2">
+        <v>100.47846889876899</v>
+      </c>
+      <c r="F115" s="2">
+        <v>49.6859504138055</v>
+      </c>
+      <c r="G115" s="2">
+        <v>76.599314125894097</v>
+      </c>
+      <c r="H115" s="2">
+        <v>53.174310065641698</v>
+      </c>
+      <c r="I115" s="2">
+        <v>65.225330227689597</v>
+      </c>
+      <c r="J115" s="2">
+        <v>64.611935951332995</v>
+      </c>
+      <c r="K115" s="2">
+        <v>69.840896865632303</v>
+      </c>
+      <c r="L115" s="2">
+        <v>69.840896865632303</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A116" s="12">
+        <v>2</v>
+      </c>
+      <c r="B116">
+        <v>26</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D116">
+        <v>60.544830159835897</v>
+      </c>
+      <c r="E116">
+        <v>97.312530969358306</v>
+      </c>
+      <c r="F116">
+        <v>68.211880774775693</v>
+      </c>
+      <c r="G116">
+        <v>89.231745277020295</v>
+      </c>
+      <c r="H116">
+        <v>55.4366155210991</v>
+      </c>
+      <c r="I116">
+        <v>51.150850376165899</v>
+      </c>
+      <c r="J116">
+        <v>62.984432080445202</v>
+      </c>
+      <c r="K116" s="1">
+        <v>69.267555022671488</v>
+      </c>
+      <c r="L116" s="1">
+        <v>69.267555022671488</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A117" s="12">
+        <v>2</v>
+      </c>
+      <c r="B117">
+        <v>27</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D117">
+        <v>75.152566035876305</v>
+      </c>
+      <c r="E117">
+        <v>86.109284842105197</v>
+      </c>
+      <c r="F117">
+        <v>55.948499003908999</v>
+      </c>
+      <c r="G117">
+        <v>96.413653806584307</v>
+      </c>
+      <c r="H117">
+        <v>46.484422395833299</v>
+      </c>
+      <c r="I117">
+        <v>50.119171090738199</v>
+      </c>
+      <c r="J117">
+        <v>68.735823362445402</v>
+      </c>
+      <c r="K117" s="1">
+        <v>68.423345791070233</v>
+      </c>
+      <c r="L117" s="1">
+        <v>68.423345791070233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A118" s="12">
+        <v>2</v>
+      </c>
+      <c r="B118">
+        <v>28</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D118">
+        <v>88.433792716520301</v>
+      </c>
+      <c r="E118">
+        <v>82.426911284210505</v>
+      </c>
+      <c r="F118">
+        <v>40.618672481101903</v>
+      </c>
+      <c r="G118">
+        <v>78.204795185185205</v>
+      </c>
+      <c r="H118">
+        <v>55.778318722197</v>
+      </c>
+      <c r="I118">
+        <v>56.729705274644999</v>
+      </c>
+      <c r="J118">
+        <v>69.8605213219993</v>
+      </c>
+      <c r="K118" s="1">
+        <v>67.436102426551315</v>
+      </c>
+      <c r="L118" s="1">
+        <v>67.436102426551315</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A119" s="12">
+        <v>2</v>
+      </c>
+      <c r="B119">
+        <v>29</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D119">
+        <v>78.7405182277938</v>
+      </c>
+      <c r="E119">
+        <v>91.168813452631497</v>
+      </c>
+      <c r="F119">
+        <v>38.4322794863563</v>
+      </c>
+      <c r="G119">
+        <v>81.966849382716006</v>
+      </c>
+      <c r="H119">
+        <v>60.559579544959597</v>
+      </c>
+      <c r="I119">
+        <v>58.008912005947202</v>
+      </c>
+      <c r="J119">
+        <v>61.222480425546401</v>
+      </c>
+      <c r="K119" s="1">
+        <v>67.157061789421533</v>
+      </c>
+      <c r="L119" s="1">
+        <v>67.157061789421533</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A120" s="12">
+        <v>2</v>
+      </c>
+      <c r="B120">
+        <v>30</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D120">
+        <v>48.627270910646899</v>
+      </c>
+      <c r="E120">
+        <v>100.481052631578</v>
+      </c>
+      <c r="F120">
+        <v>49.686947157275199</v>
+      </c>
+      <c r="G120">
+        <v>72.579745585358793</v>
+      </c>
+      <c r="H120">
+        <v>56.143651607952599</v>
+      </c>
+      <c r="I120">
+        <v>65.228409016604601</v>
+      </c>
+      <c r="J120">
+        <v>70.017363082241602</v>
+      </c>
+      <c r="K120" s="1">
+        <v>66.109205713093957</v>
+      </c>
+      <c r="L120" s="1">
+        <v>66.109205713093957</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A121" s="12">
+        <v>2</v>
+      </c>
+      <c r="B121">
+        <v>31</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D121">
+        <v>63.369565217391198</v>
+      </c>
+      <c r="E121">
+        <v>94.830940999087701</v>
+      </c>
+      <c r="F121">
+        <v>47.4103397908885</v>
+      </c>
+      <c r="G121">
+        <v>83.571829415774999</v>
+      </c>
+      <c r="H121">
+        <v>59.553872076345201</v>
+      </c>
+      <c r="I121">
+        <v>42.398973390474701</v>
+      </c>
+      <c r="J121">
+        <v>63.014614110631101</v>
+      </c>
+      <c r="K121" s="1">
+        <v>64.878590714370489</v>
+      </c>
+      <c r="L121" s="1">
+        <v>64.878590714370489</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A122" s="12">
+        <v>2</v>
+      </c>
+      <c r="B122">
+        <v>32</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D122">
+        <v>76.704826046888698</v>
+      </c>
+      <c r="E122">
+        <v>77.927734697244603</v>
+      </c>
+      <c r="F122">
+        <v>42.867197278576803</v>
+      </c>
+      <c r="G122">
+        <v>75.543242063393805</v>
+      </c>
+      <c r="H122">
+        <v>54.982599699021797</v>
+      </c>
+      <c r="I122">
+        <v>53.177805562558198</v>
+      </c>
+      <c r="J122">
+        <v>58.918084647590703</v>
+      </c>
+      <c r="K122" s="1">
+        <v>62.874498570753524</v>
+      </c>
+      <c r="L122" s="1">
+        <v>62.874498570753524</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A123" s="12">
+        <v>2</v>
+      </c>
+      <c r="B123">
+        <v>33</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D123">
+        <v>77.535558231614203</v>
+      </c>
+      <c r="E123">
+        <v>78.015780128587494</v>
+      </c>
+      <c r="F123">
+        <v>46.987186707265302</v>
+      </c>
+      <c r="G123">
+        <v>75.454447800630604</v>
+      </c>
+      <c r="H123">
+        <v>50.439892256847997</v>
+      </c>
+      <c r="I123">
+        <v>44.840409706528298</v>
+      </c>
+      <c r="J123">
+        <v>64.235128564740407</v>
+      </c>
+      <c r="K123" s="1">
+        <v>62.50120048517347</v>
+      </c>
+      <c r="L123" s="1">
+        <v>62.50120048517347</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A124" s="12">
+        <v>2</v>
+      </c>
+      <c r="B124">
+        <v>34</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D124">
+        <v>53.864919487788498</v>
+      </c>
+      <c r="E124">
+        <v>92.843157894736805</v>
+      </c>
+      <c r="F124">
+        <v>58.1973829648771</v>
+      </c>
+      <c r="G124">
+        <v>71.387757201646096</v>
+      </c>
+      <c r="H124">
+        <v>57.637206046565801</v>
+      </c>
+      <c r="I124">
+        <v>57.755126634654602</v>
+      </c>
+      <c r="J124">
+        <v>35.863984248457299</v>
+      </c>
+      <c r="K124" s="1">
+        <v>61.078504925532307</v>
+      </c>
+      <c r="L124" s="1">
+        <v>61.078504925532307</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A125" s="12">
+        <v>2</v>
+      </c>
+      <c r="B125">
+        <v>35</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D125">
+        <v>90.484683788586906</v>
+      </c>
+      <c r="E125">
+        <v>77.882232826666694</v>
+      </c>
+      <c r="F125">
+        <v>60.930503392355298</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>51.543055555555497</v>
+      </c>
+      <c r="I125">
+        <v>67.665209777884598</v>
+      </c>
+      <c r="J125">
+        <v>64.672489065502106</v>
+      </c>
+      <c r="K125" s="1">
+        <v>59.025453486650157</v>
+      </c>
+      <c r="L125" s="1">
+        <v>59.025453486650157</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A126" s="12">
+        <v>2</v>
+      </c>
+      <c r="B126">
+        <v>36</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D126">
+        <v>70.612046933451794</v>
+      </c>
+      <c r="E126">
+        <v>103.763262634469</v>
+      </c>
+      <c r="F126">
+        <v>27.367389737132399</v>
+      </c>
+      <c r="G126">
+        <v>91.529357855804406</v>
+      </c>
+      <c r="H126">
+        <v>29.1724411012583</v>
+      </c>
+      <c r="I126">
+        <v>23.2477845292761</v>
+      </c>
+      <c r="J126">
+        <v>33.647666053269802</v>
+      </c>
+      <c r="K126" s="1">
+        <v>54.191421263523111</v>
+      </c>
+      <c r="L126" s="1">
+        <v>54.191421263523111</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A127" s="12">
+        <v>2</v>
+      </c>
+      <c r="B127">
+        <v>37</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D127">
+        <v>66.767326086956501</v>
+      </c>
+      <c r="E127">
+        <v>65.936842105263096</v>
+      </c>
+      <c r="F127">
+        <v>39.495123966942103</v>
+      </c>
+      <c r="G127">
+        <v>64.0187522485584</v>
+      </c>
+      <c r="H127">
+        <v>34.266979166666601</v>
+      </c>
+      <c r="I127">
+        <v>38.082475533929802</v>
+      </c>
+      <c r="J127">
+        <v>47.715886804249699</v>
+      </c>
+      <c r="K127" s="1">
+        <v>50.897626558938029</v>
+      </c>
+      <c r="L127" s="1">
+        <v>50.897626558938029</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A128" s="12">
+        <v>2</v>
+      </c>
+      <c r="B128">
+        <v>38</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D128">
+        <v>49.179204449851703</v>
+      </c>
+      <c r="E128">
+        <v>51.929828503395697</v>
+      </c>
+      <c r="F128">
+        <v>42.9700909475998</v>
+      </c>
+      <c r="G128">
+        <v>49.190745227243397</v>
+      </c>
+      <c r="H128">
+        <v>50.004416442641102</v>
+      </c>
+      <c r="I128">
+        <v>48.9121211828149</v>
+      </c>
+      <c r="J128">
+        <v>45.1043716232939</v>
+      </c>
+      <c r="K128" s="1">
+        <v>48.18439691097722</v>
+      </c>
+      <c r="L128" s="1">
+        <v>48.18439691097722</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A129" s="12">
+        <v>2</v>
+      </c>
+      <c r="B129">
+        <v>39</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D129">
+        <v>50.880434782608603</v>
+      </c>
+      <c r="E129">
+        <v>50.463859649122703</v>
+      </c>
+      <c r="F129">
+        <v>24.2424242424242</v>
+      </c>
+      <c r="G129">
+        <v>45.016460905349703</v>
+      </c>
+      <c r="H129">
+        <v>23.4027777777777</v>
+      </c>
+      <c r="I129">
+        <v>26.7094017094017</v>
+      </c>
+      <c r="J129">
+        <v>28.602620087336199</v>
+      </c>
+      <c r="K129" s="1">
+        <v>35.616854164860115</v>
+      </c>
+      <c r="L129" s="1">
+        <v>35.616854164860115</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A130" s="12">
+        <v>2</v>
+      </c>
+      <c r="B130">
+        <v>40</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D130">
+        <v>61.296093553276698</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>44.093529115072698</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130">
+        <v>0</v>
+      </c>
+      <c r="J130">
+        <v>59.4036932763808</v>
+      </c>
+      <c r="K130" s="1">
+        <v>23.5419022778186</v>
+      </c>
+      <c r="L130" s="1">
+        <v>23.5419022778186</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:L49">
     <sortCondition descending="1" ref="L1:L49"/>

</xml_diff>